<commit_message>
Bugfixes, improved sorting, and more
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="40" windowWidth="28800" windowHeight="15940" tabRatio="750" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18040" tabRatio="750" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PO" sheetId="16" r:id="rId1"/>
     <sheet name="CO" sheetId="3" r:id="rId2"/>
     <sheet name="Grades" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="20" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
     <t>Student ID</t>
   </si>
@@ -201,9 +200,6 @@
     <t>2. Analyze the problems and develop basic computer algorithms</t>
   </si>
   <si>
-    <t>P12</t>
-  </si>
-  <si>
     <t>3. Create computer programs to solve engineering problems</t>
   </si>
   <si>
@@ -360,7 +356,10 @@
     <t xml:space="preserve">CO2, CO3, </t>
   </si>
   <si>
-    <t>Question Course Outcomes:</t>
+    <t>PO1,PO2,PO4,PO6,PO9,PO12</t>
+  </si>
+  <si>
+    <t>Related Course Outcomes:</t>
   </si>
 </sst>
 </file>
@@ -508,8 +507,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="207">
+  <cellStyleXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -758,11 +761,11 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,7 +773,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="207">
+  <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -874,6 +877,8 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -977,6 +982,8 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1317,7 +1324,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1465,25 +1472,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="57.83203125" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25">
+    <row r="1" spans="1:6" ht="25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20">
+    <row r="2" spans="1:6" ht="20">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1504,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1508,7 +1515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1516,70 +1523,40 @@
         <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1575,7 @@
   <dimension ref="A1:AM34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1622,76 +1599,76 @@
     <row r="2" spans="1:39" ht="25">
       <c r="B2" s="3"/>
       <c r="D2" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16" t="s">
+      <c r="M2" s="18"/>
+      <c r="N2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
       <c r="T2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="16"/>
+      <c r="V2" s="18"/>
       <c r="W2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16" t="s">
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
     </row>
     <row r="3" spans="1:39" ht="20">
       <c r="D3" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="19">
         <v>1.25</v>
@@ -1761,114 +1738,114 @@
     <row r="4" spans="1:39" ht="25">
       <c r="B4" s="3"/>
       <c r="D4" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="18">
-        <v>1</v>
-      </c>
-      <c r="G4" s="18">
+        <v>99</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17">
         <v>2</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <v>3</v>
       </c>
-      <c r="I4" s="18">
-        <v>1</v>
-      </c>
-      <c r="J4" s="18">
+      <c r="I4" s="17">
+        <v>1</v>
+      </c>
+      <c r="J4" s="17">
         <v>2</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="17">
         <v>3</v>
       </c>
-      <c r="L4" s="18">
-        <v>1</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="L4" s="17">
+        <v>1</v>
+      </c>
+      <c r="M4" s="17">
         <v>2</v>
       </c>
-      <c r="N4" s="18">
-        <v>1</v>
-      </c>
-      <c r="O4" s="18">
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17">
         <v>2</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="17">
         <v>3</v>
       </c>
-      <c r="Q4" s="18">
-        <v>1</v>
-      </c>
-      <c r="R4" s="18">
+      <c r="Q4" s="17">
+        <v>1</v>
+      </c>
+      <c r="R4" s="17">
         <v>2</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S4" s="17">
         <v>3</v>
       </c>
-      <c r="T4" s="18">
-        <v>1</v>
-      </c>
-      <c r="U4" s="18">
-        <v>1</v>
-      </c>
-      <c r="V4" s="18">
+      <c r="T4" s="17">
+        <v>1</v>
+      </c>
+      <c r="U4" s="17">
+        <v>1</v>
+      </c>
+      <c r="V4" s="17">
         <v>2</v>
       </c>
-      <c r="W4" s="18">
-        <v>1</v>
-      </c>
-      <c r="X4" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="18">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="18">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="18">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="18">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="18">
+      <c r="W4" s="17">
+        <v>1</v>
+      </c>
+      <c r="X4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="17">
         <v>2</v>
       </c>
-      <c r="AD4" s="18">
+      <c r="AD4" s="17">
         <v>3</v>
       </c>
-      <c r="AE4" s="18">
+      <c r="AE4" s="17">
         <v>4</v>
       </c>
-      <c r="AF4" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="18">
+      <c r="AF4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="17">
         <v>2</v>
       </c>
-      <c r="AH4" s="18">
+      <c r="AH4" s="17">
         <v>3</v>
       </c>
-      <c r="AI4" s="18">
+      <c r="AI4" s="17">
         <v>4</v>
       </c>
-      <c r="AJ4" s="18">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="18">
+      <c r="AJ4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="17">
         <v>2</v>
       </c>
-      <c r="AL4" s="18">
+      <c r="AL4" s="17">
         <v>3</v>
       </c>
-      <c r="AM4" s="18">
+      <c r="AM4" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="20">
       <c r="D5" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="5">
         <v>30</v>
@@ -1984,16 +1961,16 @@
         <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="K6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>10</v>
@@ -2002,46 +1979,46 @@
         <v>11</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="S6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="T6" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="X6" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="X6" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="Y6" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>13</v>
@@ -2050,40 +2027,40 @@
         <v>13</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AI6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="7" spans="1:39" ht="20">
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -2199,18 +2176,154 @@
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F9" s="8">
+        <f>F4</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" ref="G9:AM9" si="0">G4</f>
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AB9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AD9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AE9" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AF9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AG9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AH9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AI9" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AJ9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AK9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AL9" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AM9" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:39">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -2241,6 +2354,15 @@
       </c>
       <c r="M10">
         <v>10</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2317,7 +2439,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -2433,7 +2555,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -2549,13 +2671,13 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2579,6 +2701,15 @@
         <v>0</v>
       </c>
       <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
@@ -2656,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -2772,7 +2903,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -2888,7 +3019,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -3004,13 +3135,13 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17">
         <v>20</v>
@@ -3120,13 +3251,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3236,7 +3367,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -3320,6 +3451,18 @@
         <v>0</v>
       </c>
       <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
         <v>0</v>
       </c>
       <c r="AJ19">
@@ -3340,7 +3483,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -3456,13 +3599,13 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21">
         <v>30</v>
@@ -3572,7 +3715,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -3688,13 +3831,13 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -3804,7 +3947,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -3920,7 +4063,7 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -4004,6 +4147,18 @@
         <v>0</v>
       </c>
       <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
         <v>0</v>
       </c>
       <c r="AJ25">
@@ -4024,7 +4179,7 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -4140,7 +4295,7 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -4256,7 +4411,7 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -4372,7 +4527,7 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -4488,7 +4643,7 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -4572,6 +4727,18 @@
         <v>0</v>
       </c>
       <c r="AE30">
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
         <v>0</v>
       </c>
       <c r="AJ30">
@@ -4592,7 +4759,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -4677,6 +4844,18 @@
       </c>
       <c r="AE31">
         <v>2</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
       </c>
       <c r="AJ31">
         <v>10</v>
@@ -4696,13 +4875,13 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -4812,7 +4991,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -4896,6 +5075,18 @@
         <v>0</v>
       </c>
       <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
         <v>0</v>
       </c>
       <c r="AJ33">
@@ -4916,7 +5107,7 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -5000,6 +5191,18 @@
         <v>0</v>
       </c>
       <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
         <v>0</v>
       </c>
       <c r="AJ34">
@@ -5044,67 +5247,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="2" spans="1:4">
-      <c r="B2">
-        <v>0.3</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <f>SUMPRODUCT(B2:D2,B3:D3,B5:D5)</f>
-        <v>51.2</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="str">
-        <f ca="1">IF($A10="","",ROUND(100*SUMPRODUCT(INDIRECT(#REF!),INDIRECT(#REF!),--INDIRECT(#REF!))/SUMPRODUCT(INDIRECT(#REF!),INDIRECT(#REF!),--INDIRECT(#REF!)),2))</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed implementation with Excel output
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18040" tabRatio="750" activeTab="2"/>
+    <workbookView xWindow="32740" yWindow="100" windowWidth="28800" windowHeight="18160" tabRatio="750" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="PO" sheetId="16" r:id="rId1"/>
-    <sheet name="CO" sheetId="3" r:id="rId2"/>
+    <sheet name="Program" sheetId="16" r:id="rId1"/>
+    <sheet name="Course" sheetId="3" r:id="rId2"/>
     <sheet name="Grades" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="120">
   <si>
     <t>Student ID</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>Module 1 : Course Outcome List</t>
-  </si>
-  <si>
     <t>Course Outcomes</t>
   </si>
   <si>
@@ -359,14 +356,38 @@
     <t>PO1,PO2,PO4,PO6,PO9,PO12</t>
   </si>
   <si>
-    <t>Related Course Outcomes:</t>
+    <t>Course Name:</t>
+  </si>
+  <si>
+    <t>Course Code:</t>
+  </si>
+  <si>
+    <t>Course ECTS Credit:</t>
+  </si>
+  <si>
+    <t>Course US Credit:</t>
+  </si>
+  <si>
+    <t>COMP103</t>
+  </si>
+  <si>
+    <t>Computer Programming</t>
+  </si>
+  <si>
+    <t>Related Outcomes:</t>
+  </si>
+  <si>
+    <t>Cem Gokmen</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -442,6 +463,19 @@
       <color rgb="FF222426"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -507,7 +541,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="211">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -719,8 +753,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -763,6 +799,13 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,8 +815,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="211">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -879,6 +928,7 @@
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -984,6 +1034,7 @@
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1324,7 +1375,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1335,128 +1386,128 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" ht="49" thickTop="1">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="80">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="49" thickBot="1">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" thickTop="1" thickBot="1">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" thickTop="1" thickBot="1">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="50" thickTop="1" thickBot="1">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" ht="16" thickTop="1"/>
@@ -1472,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1485,78 +1536,105 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20">
-      <c r="A2" s="1" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="C8" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="C9" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="C10" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
+      <c r="C11" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1572,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM34"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AD39" sqref="AD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1592,115 +1670,115 @@
   <sheetData>
     <row r="1" spans="1:39" ht="25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:39" ht="25">
       <c r="B2" s="3"/>
       <c r="D2" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18" t="s">
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18" t="s">
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" s="18"/>
+      <c r="V2" s="21"/>
       <c r="W2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK2" s="21"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
     </row>
     <row r="3" spans="1:39" ht="20">
       <c r="D3" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="19">
+        <v>99</v>
+      </c>
+      <c r="F3" s="22">
         <v>1.25</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23">
         <v>1.25</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="19">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="22">
         <v>1.25</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19">
+      <c r="M3" s="22"/>
+      <c r="N3" s="22">
         <v>1.25</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22">
         <v>1.25</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
       <c r="T3" s="4">
         <v>1.25</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="22">
         <v>1.25</v>
       </c>
-      <c r="V3" s="19"/>
+      <c r="V3" s="22"/>
       <c r="W3" s="4">
         <v>1.25</v>
       </c>
@@ -1716,29 +1794,29 @@
       <c r="AA3" s="4">
         <v>5</v>
       </c>
-      <c r="AB3" s="19">
+      <c r="AB3" s="22">
         <v>15</v>
       </c>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19">
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22">
         <v>15</v>
       </c>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19"/>
-      <c r="AJ3" s="19">
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22">
         <v>40</v>
       </c>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="19"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="22"/>
     </row>
     <row r="4" spans="1:39" ht="25">
       <c r="B4" s="3"/>
       <c r="D4" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="17">
         <v>1</v>
@@ -1845,7 +1923,7 @@
     </row>
     <row r="5" spans="1:39" ht="20">
       <c r="D5" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="5">
         <v>30</v>
@@ -1952,115 +2030,115 @@
     </row>
     <row r="6" spans="1:39" ht="20">
       <c r="D6" s="14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="N6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="T6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S6" s="5" t="s">
+      <c r="AF6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="T6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="W6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="X6" s="5" t="s">
+      <c r="AJ6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="Y6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AM6" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AL6" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="20">
       <c r="C7" s="16"/>
       <c r="D7" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -2173,13 +2251,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="8">
         <f>F4</f>
@@ -2323,13 +2401,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>30</v>
@@ -2439,13 +2517,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>30</v>
@@ -2555,13 +2633,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12">
         <v>30</v>
@@ -2671,13 +2749,13 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2787,13 +2865,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -2903,13 +2981,13 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -3019,13 +3097,13 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -3135,13 +3213,13 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17">
         <v>20</v>
@@ -3251,13 +3329,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3367,13 +3445,13 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -3483,13 +3561,13 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -3599,13 +3677,13 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21">
         <v>30</v>
@@ -3715,13 +3793,13 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -3831,13 +3909,13 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -3947,13 +4025,13 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24">
         <v>20</v>
@@ -4063,13 +4141,13 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -4179,13 +4257,13 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -4295,13 +4373,13 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -4411,13 +4489,13 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28">
         <v>30</v>
@@ -4527,13 +4605,13 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -4643,13 +4721,13 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30">
         <v>20</v>
@@ -4759,13 +4837,13 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -4875,13 +4953,13 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32">
         <v>10</v>
@@ -4991,13 +5069,13 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -5107,13 +5185,13 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -5216,6 +5294,122 @@
       </c>
       <c r="AM34">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="24">
+        <v>30</v>
+      </c>
+      <c r="G35" s="24">
+        <v>25</v>
+      </c>
+      <c r="H35" s="24">
+        <v>45</v>
+      </c>
+      <c r="I35" s="24">
+        <v>30</v>
+      </c>
+      <c r="J35" s="24">
+        <v>50</v>
+      </c>
+      <c r="K35" s="24">
+        <v>20</v>
+      </c>
+      <c r="L35" s="24">
+        <v>30</v>
+      </c>
+      <c r="M35" s="24">
+        <v>70</v>
+      </c>
+      <c r="N35" s="24">
+        <v>40</v>
+      </c>
+      <c r="O35" s="24">
+        <v>30</v>
+      </c>
+      <c r="P35" s="24">
+        <v>30</v>
+      </c>
+      <c r="Q35" s="24">
+        <v>30</v>
+      </c>
+      <c r="R35" s="24">
+        <v>30</v>
+      </c>
+      <c r="S35" s="24">
+        <v>40</v>
+      </c>
+      <c r="T35" s="24">
+        <v>100</v>
+      </c>
+      <c r="U35" s="24">
+        <v>70</v>
+      </c>
+      <c r="V35" s="24">
+        <v>30</v>
+      </c>
+      <c r="W35" s="24">
+        <v>100</v>
+      </c>
+      <c r="X35" s="24">
+        <v>100</v>
+      </c>
+      <c r="Y35" s="25">
+        <v>100</v>
+      </c>
+      <c r="Z35" s="25">
+        <v>100</v>
+      </c>
+      <c r="AA35" s="25">
+        <v>100</v>
+      </c>
+      <c r="AB35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AC35" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AE35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AF35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AG35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AH35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AI35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AJ35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AK35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AL35" s="25">
+        <v>25</v>
+      </c>
+      <c r="AM35" s="25">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>